<commit_message>
more strats for sw.
</commit_message>
<xml_diff>
--- a/strats-sources/spaceWolvesStrats.xlsx
+++ b/strats-sources/spaceWolvesStrats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micro\gitrepos\w40k-strat-card\strats-sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E69A56-4E5A-4688-9967-A26A3E14A082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{799EBB89-C2BD-4447-8E8E-0C9F36CA0BBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3DE3896D-95B2-400C-96E2-85A96F1479CA}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="40">
   <si>
     <t>Timing</t>
   </si>
@@ -142,10 +142,19 @@
     <t>Only in death, duty ends</t>
   </si>
   <si>
-    <t>Phase de combat, une figurine est détruite</t>
-  </si>
-  <si>
     <t>Si une figurine n'a pas &amp;eacute;t&amp;eacute; s&amp;eacute;lectionn&amp;eacute; pour combattre dans cette phase est d&amp;eacute;truite. Ne pas retirer la figurine, elle peut combattre apr&amp;egrave;s que la figurine attaquante &amp;agrave; terminer de faire ses attaques.&lt;br/&gt;La figurine est ensuite retir&amp;eacute;e.</t>
+  </si>
+  <si>
+    <t>Toutes phases</t>
+  </si>
+  <si>
+    <t>Deed worthy saga</t>
+  </si>
+  <si>
+    <t>Lorsqu'un personnage space wolf autre que le seigneur de guerre satisfait les pré requis d'une saga, celui ci b&amp;eacute;n&amp;eacute;ficie des effets de celle ci jusqu'&amp;agrave; la fin de la saga.</t>
+  </si>
+  <si>
+    <t>Phase de combat, une figurine est d&amp;eacute;truite</t>
   </si>
 </sst>
 </file>
@@ -503,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0B88374-B535-46D0-A48E-0EFF11686FCD}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="59.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,10 +739,10 @@
         <v>34</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>8</v>
@@ -749,6 +758,29 @@
       </c>
       <c r="H9" s="1" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>